<commit_message>
Maybe changed some references while copying footprints for updated version
</commit_message>
<xml_diff>
--- a/Fabrication/ISO_Power_PCB/BOM_ISO_Power_PCB_final.xlsx
+++ b/Fabrication/ISO_Power_PCB/BOM_ISO_Power_PCB_final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheard\Documents\KiCad\Projects\ISOpower\Fabrication\ISO_Power_PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheard\Documents\0000.KiCad\Projects\001-remotelabs\ISOpower\Fabrication\ISO_Power_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1"/>
 </workbook>
 </file>
 
@@ -996,6 +996,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1006,9 +1009,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1361,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX559"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1385,23 +1385,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="1:50" ht="25.7" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -1440,7 +1440,7 @@
       <c r="L2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="16" t="s">
         <v>233</v>
       </c>
       <c r="N2" s="6" t="s">

</xml_diff>